<commit_message>
md files from rmd scripts
</commit_message>
<xml_diff>
--- a/data/BLASToutput/Taxonomic_assignment/Choice_required_GMGI_multiplehits.xlsx
+++ b/data/BLASToutput/Taxonomic_assignment/Choice_required_GMGI_multiplehits.xlsx
@@ -1550,7 +1550,7 @@
         <v>168</v>
       </c>
       <c r="G17">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H17">
         <v>107</v>
@@ -1621,7 +1621,7 @@
         <v>168</v>
       </c>
       <c r="G18">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H18">
         <v>107</v>
@@ -1692,7 +1692,7 @@
         <v>168</v>
       </c>
       <c r="G19">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="H19">
         <v>107</v>
@@ -3609,7 +3609,7 @@
         <v>12</v>
       </c>
       <c r="G46">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="H46">
         <v>108</v>
@@ -3680,7 +3680,7 @@
         <v>12</v>
       </c>
       <c r="G47">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="H47">
         <v>108</v>
@@ -3751,7 +3751,7 @@
         <v>12</v>
       </c>
       <c r="G48">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="H48">
         <v>107</v>
@@ -3822,7 +3822,7 @@
         <v>12</v>
       </c>
       <c r="G49">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="H49">
         <v>108</v>

</xml_diff>